<commit_message>
editted days im away
</commit_message>
<xml_diff>
--- a/Information/May Calendar.xlsx
+++ b/Information/May Calendar.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andif\Desktop\Shift Course\Project-1\Information\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D83E1BF-CD1E-4C32-9155-2847CEA6979E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26221"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{77ABF995-AB93-4BCC-8C53-946F31CCA3A9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14420"/>
   </bookViews>
   <sheets>
     <sheet name="Wednesday" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -25,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
   <si>
     <t>Monday</t>
   </si>
@@ -96,7 +93,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -134,11 +131,11 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -147,7 +144,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -155,56 +152,56 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -213,60 +210,60 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -274,10 +271,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -285,10 +282,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -296,40 +293,40 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -437,7 +434,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{2F65F7AE-5C10-49AC-8717-BA516AD2F7A7}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -496,7 +493,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -548,7 +545,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -742,89 +739,89 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA7DAF1-8E4B-4296-ABC0-616DAF2BDF69}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="8" width="15.26953125" customWidth="1"/>
-    <col min="258" max="264" width="15.26953125" customWidth="1"/>
-    <col min="514" max="520" width="15.26953125" customWidth="1"/>
-    <col min="770" max="776" width="15.26953125" customWidth="1"/>
-    <col min="1026" max="1032" width="15.26953125" customWidth="1"/>
-    <col min="1282" max="1288" width="15.26953125" customWidth="1"/>
-    <col min="1538" max="1544" width="15.26953125" customWidth="1"/>
-    <col min="1794" max="1800" width="15.26953125" customWidth="1"/>
-    <col min="2050" max="2056" width="15.26953125" customWidth="1"/>
-    <col min="2306" max="2312" width="15.26953125" customWidth="1"/>
-    <col min="2562" max="2568" width="15.26953125" customWidth="1"/>
-    <col min="2818" max="2824" width="15.26953125" customWidth="1"/>
-    <col min="3074" max="3080" width="15.26953125" customWidth="1"/>
-    <col min="3330" max="3336" width="15.26953125" customWidth="1"/>
-    <col min="3586" max="3592" width="15.26953125" customWidth="1"/>
-    <col min="3842" max="3848" width="15.26953125" customWidth="1"/>
-    <col min="4098" max="4104" width="15.26953125" customWidth="1"/>
-    <col min="4354" max="4360" width="15.26953125" customWidth="1"/>
-    <col min="4610" max="4616" width="15.26953125" customWidth="1"/>
-    <col min="4866" max="4872" width="15.26953125" customWidth="1"/>
-    <col min="5122" max="5128" width="15.26953125" customWidth="1"/>
-    <col min="5378" max="5384" width="15.26953125" customWidth="1"/>
-    <col min="5634" max="5640" width="15.26953125" customWidth="1"/>
-    <col min="5890" max="5896" width="15.26953125" customWidth="1"/>
-    <col min="6146" max="6152" width="15.26953125" customWidth="1"/>
-    <col min="6402" max="6408" width="15.26953125" customWidth="1"/>
-    <col min="6658" max="6664" width="15.26953125" customWidth="1"/>
-    <col min="6914" max="6920" width="15.26953125" customWidth="1"/>
-    <col min="7170" max="7176" width="15.26953125" customWidth="1"/>
-    <col min="7426" max="7432" width="15.26953125" customWidth="1"/>
-    <col min="7682" max="7688" width="15.26953125" customWidth="1"/>
-    <col min="7938" max="7944" width="15.26953125" customWidth="1"/>
-    <col min="8194" max="8200" width="15.26953125" customWidth="1"/>
-    <col min="8450" max="8456" width="15.26953125" customWidth="1"/>
-    <col min="8706" max="8712" width="15.26953125" customWidth="1"/>
-    <col min="8962" max="8968" width="15.26953125" customWidth="1"/>
-    <col min="9218" max="9224" width="15.26953125" customWidth="1"/>
-    <col min="9474" max="9480" width="15.26953125" customWidth="1"/>
-    <col min="9730" max="9736" width="15.26953125" customWidth="1"/>
-    <col min="9986" max="9992" width="15.26953125" customWidth="1"/>
-    <col min="10242" max="10248" width="15.26953125" customWidth="1"/>
-    <col min="10498" max="10504" width="15.26953125" customWidth="1"/>
-    <col min="10754" max="10760" width="15.26953125" customWidth="1"/>
-    <col min="11010" max="11016" width="15.26953125" customWidth="1"/>
-    <col min="11266" max="11272" width="15.26953125" customWidth="1"/>
-    <col min="11522" max="11528" width="15.26953125" customWidth="1"/>
-    <col min="11778" max="11784" width="15.26953125" customWidth="1"/>
-    <col min="12034" max="12040" width="15.26953125" customWidth="1"/>
-    <col min="12290" max="12296" width="15.26953125" customWidth="1"/>
-    <col min="12546" max="12552" width="15.26953125" customWidth="1"/>
-    <col min="12802" max="12808" width="15.26953125" customWidth="1"/>
-    <col min="13058" max="13064" width="15.26953125" customWidth="1"/>
-    <col min="13314" max="13320" width="15.26953125" customWidth="1"/>
-    <col min="13570" max="13576" width="15.26953125" customWidth="1"/>
-    <col min="13826" max="13832" width="15.26953125" customWidth="1"/>
-    <col min="14082" max="14088" width="15.26953125" customWidth="1"/>
-    <col min="14338" max="14344" width="15.26953125" customWidth="1"/>
-    <col min="14594" max="14600" width="15.26953125" customWidth="1"/>
-    <col min="14850" max="14856" width="15.26953125" customWidth="1"/>
-    <col min="15106" max="15112" width="15.26953125" customWidth="1"/>
-    <col min="15362" max="15368" width="15.26953125" customWidth="1"/>
-    <col min="15618" max="15624" width="15.26953125" customWidth="1"/>
-    <col min="15874" max="15880" width="15.26953125" customWidth="1"/>
-    <col min="16130" max="16136" width="15.26953125" customWidth="1"/>
+    <col min="2" max="8" width="15.33203125" customWidth="1"/>
+    <col min="258" max="264" width="15.33203125" customWidth="1"/>
+    <col min="514" max="520" width="15.33203125" customWidth="1"/>
+    <col min="770" max="776" width="15.33203125" customWidth="1"/>
+    <col min="1026" max="1032" width="15.33203125" customWidth="1"/>
+    <col min="1282" max="1288" width="15.33203125" customWidth="1"/>
+    <col min="1538" max="1544" width="15.33203125" customWidth="1"/>
+    <col min="1794" max="1800" width="15.33203125" customWidth="1"/>
+    <col min="2050" max="2056" width="15.33203125" customWidth="1"/>
+    <col min="2306" max="2312" width="15.33203125" customWidth="1"/>
+    <col min="2562" max="2568" width="15.33203125" customWidth="1"/>
+    <col min="2818" max="2824" width="15.33203125" customWidth="1"/>
+    <col min="3074" max="3080" width="15.33203125" customWidth="1"/>
+    <col min="3330" max="3336" width="15.33203125" customWidth="1"/>
+    <col min="3586" max="3592" width="15.33203125" customWidth="1"/>
+    <col min="3842" max="3848" width="15.33203125" customWidth="1"/>
+    <col min="4098" max="4104" width="15.33203125" customWidth="1"/>
+    <col min="4354" max="4360" width="15.33203125" customWidth="1"/>
+    <col min="4610" max="4616" width="15.33203125" customWidth="1"/>
+    <col min="4866" max="4872" width="15.33203125" customWidth="1"/>
+    <col min="5122" max="5128" width="15.33203125" customWidth="1"/>
+    <col min="5378" max="5384" width="15.33203125" customWidth="1"/>
+    <col min="5634" max="5640" width="15.33203125" customWidth="1"/>
+    <col min="5890" max="5896" width="15.33203125" customWidth="1"/>
+    <col min="6146" max="6152" width="15.33203125" customWidth="1"/>
+    <col min="6402" max="6408" width="15.33203125" customWidth="1"/>
+    <col min="6658" max="6664" width="15.33203125" customWidth="1"/>
+    <col min="6914" max="6920" width="15.33203125" customWidth="1"/>
+    <col min="7170" max="7176" width="15.33203125" customWidth="1"/>
+    <col min="7426" max="7432" width="15.33203125" customWidth="1"/>
+    <col min="7682" max="7688" width="15.33203125" customWidth="1"/>
+    <col min="7938" max="7944" width="15.33203125" customWidth="1"/>
+    <col min="8194" max="8200" width="15.33203125" customWidth="1"/>
+    <col min="8450" max="8456" width="15.33203125" customWidth="1"/>
+    <col min="8706" max="8712" width="15.33203125" customWidth="1"/>
+    <col min="8962" max="8968" width="15.33203125" customWidth="1"/>
+    <col min="9218" max="9224" width="15.33203125" customWidth="1"/>
+    <col min="9474" max="9480" width="15.33203125" customWidth="1"/>
+    <col min="9730" max="9736" width="15.33203125" customWidth="1"/>
+    <col min="9986" max="9992" width="15.33203125" customWidth="1"/>
+    <col min="10242" max="10248" width="15.33203125" customWidth="1"/>
+    <col min="10498" max="10504" width="15.33203125" customWidth="1"/>
+    <col min="10754" max="10760" width="15.33203125" customWidth="1"/>
+    <col min="11010" max="11016" width="15.33203125" customWidth="1"/>
+    <col min="11266" max="11272" width="15.33203125" customWidth="1"/>
+    <col min="11522" max="11528" width="15.33203125" customWidth="1"/>
+    <col min="11778" max="11784" width="15.33203125" customWidth="1"/>
+    <col min="12034" max="12040" width="15.33203125" customWidth="1"/>
+    <col min="12290" max="12296" width="15.33203125" customWidth="1"/>
+    <col min="12546" max="12552" width="15.33203125" customWidth="1"/>
+    <col min="12802" max="12808" width="15.33203125" customWidth="1"/>
+    <col min="13058" max="13064" width="15.33203125" customWidth="1"/>
+    <col min="13314" max="13320" width="15.33203125" customWidth="1"/>
+    <col min="13570" max="13576" width="15.33203125" customWidth="1"/>
+    <col min="13826" max="13832" width="15.33203125" customWidth="1"/>
+    <col min="14082" max="14088" width="15.33203125" customWidth="1"/>
+    <col min="14338" max="14344" width="15.33203125" customWidth="1"/>
+    <col min="14594" max="14600" width="15.33203125" customWidth="1"/>
+    <col min="14850" max="14856" width="15.33203125" customWidth="1"/>
+    <col min="15106" max="15112" width="15.33203125" customWidth="1"/>
+    <col min="15362" max="15368" width="15.33203125" customWidth="1"/>
+    <col min="15618" max="15624" width="15.33203125" customWidth="1"/>
+    <col min="15874" max="15880" width="15.33203125" customWidth="1"/>
+    <col min="16130" max="16136" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="13" thickBot="1">
       <c r="B1" s="25" t="s">
         <v>13</v>
       </c>
@@ -835,7 +832,7 @@
       <c r="G1" s="26"/>
       <c r="H1" s="27"/>
     </row>
-    <row r="2" spans="1:8" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="13" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -858,7 +855,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -882,7 +879,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -894,7 +891,7 @@
       <c r="G4" s="21"/>
       <c r="H4" s="22"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -906,7 +903,7 @@
       <c r="G5" s="21"/>
       <c r="H5" s="22"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -918,7 +915,7 @@
       <c r="G6" s="21"/>
       <c r="H6" s="22"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -930,7 +927,7 @@
       <c r="G7" s="21"/>
       <c r="H7" s="22"/>
     </row>
-    <row r="8" spans="1:8" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="13" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -942,7 +939,7 @@
       <c r="G8" s="23"/>
       <c r="H8" s="24"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -968,7 +965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -984,19 +981,23 @@
       <c r="G10" s="21"/>
       <c r="H10" s="22"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="E11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="G11" s="21"/>
       <c r="H11" s="22"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1010,7 +1011,7 @@
       <c r="G12" s="21"/>
       <c r="H12" s="22"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1022,7 +1023,7 @@
       <c r="G13" s="21"/>
       <c r="H13" s="22"/>
     </row>
-    <row r="14" spans="1:8" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="13" thickBot="1">
       <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
@@ -1034,7 +1035,7 @@
       <c r="G14" s="23"/>
       <c r="H14" s="24"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
@@ -1060,7 +1061,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="5" t="s">
         <v>8</v>
       </c>
@@ -1076,7 +1077,7 @@
       <c r="G16" s="21"/>
       <c r="H16" s="22"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
@@ -1088,7 +1089,7 @@
       <c r="G17" s="21"/>
       <c r="H17" s="22"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="5" t="s">
         <v>10</v>
       </c>
@@ -1102,7 +1103,7 @@
       <c r="G18" s="21"/>
       <c r="H18" s="22"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="5" t="s">
         <v>11</v>
       </c>
@@ -1114,7 +1115,7 @@
       <c r="G19" s="21"/>
       <c r="H19" s="22"/>
     </row>
-    <row r="20" spans="1:8" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="13" thickBot="1">
       <c r="A20" s="6" t="s">
         <v>12</v>
       </c>
@@ -1126,7 +1127,7 @@
       <c r="G20" s="23"/>
       <c r="H20" s="24"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1152,7 +1153,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -1166,7 +1167,7 @@
       <c r="G22" s="21"/>
       <c r="H22" s="22"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="5" t="s">
         <v>9</v>
       </c>
@@ -1178,7 +1179,7 @@
       <c r="G23" s="21"/>
       <c r="H23" s="22"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="5" t="s">
         <v>10</v>
       </c>
@@ -1190,7 +1191,7 @@
       <c r="G24" s="21"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="5" t="s">
         <v>11</v>
       </c>
@@ -1202,7 +1203,7 @@
       <c r="G25" s="21"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:8" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="13" thickBot="1">
       <c r="A26" s="6" t="s">
         <v>12</v>
       </c>
@@ -1214,7 +1215,7 @@
       <c r="G26" s="23"/>
       <c r="H26" s="24"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="4" t="s">
         <v>7</v>
       </c>
@@ -1236,7 +1237,7 @@
       <c r="G27" s="8"/>
       <c r="H27" s="9"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="5" t="s">
         <v>8</v>
       </c>
@@ -1250,7 +1251,7 @@
       <c r="G28" s="11"/>
       <c r="H28" s="12"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="5" t="s">
         <v>9</v>
       </c>
@@ -1262,7 +1263,7 @@
       <c r="G29" s="11"/>
       <c r="H29" s="12"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="5" t="s">
         <v>10</v>
       </c>
@@ -1276,7 +1277,7 @@
       <c r="G30" s="11"/>
       <c r="H30" s="12"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="5" t="s">
         <v>11</v>
       </c>
@@ -1288,7 +1289,7 @@
       <c r="G31" s="11"/>
       <c r="H31" s="12"/>
     </row>
-    <row r="32" spans="1:8" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="13" thickBot="1">
       <c r="A32" s="6" t="s">
         <v>12</v>
       </c>
@@ -1306,7 +1307,12 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.15748031496062992" header="0.19685039370078741" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="130" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="130" orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Nhan inputs leave for Wed
Nhan inputs leave for Wed
</commit_message>
<xml_diff>
--- a/Information/May Calendar.xlsx
+++ b/Information/May Calendar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andif\Desktop\Shift Course\Project-1\Information\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaph\Documents\GitHub\Project-1\Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D83E1BF-CD1E-4C32-9155-2847CEA6979E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E44A28-6935-4AEB-9E96-BDAC46CF4030}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{77ABF995-AB93-4BCC-8C53-946F31CCA3A9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{77ABF995-AB93-4BCC-8C53-946F31CCA3A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Wednesday" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>Monday</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>In at 12ish</t>
+  </si>
+  <si>
+    <t>Leave at 3:00pm</t>
   </si>
 </sst>
 </file>
@@ -752,79 +755,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA7DAF1-8E4B-4296-ABC0-616DAF2BDF69}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="8" width="15.26953125" customWidth="1"/>
-    <col min="258" max="264" width="15.26953125" customWidth="1"/>
-    <col min="514" max="520" width="15.26953125" customWidth="1"/>
-    <col min="770" max="776" width="15.26953125" customWidth="1"/>
-    <col min="1026" max="1032" width="15.26953125" customWidth="1"/>
-    <col min="1282" max="1288" width="15.26953125" customWidth="1"/>
-    <col min="1538" max="1544" width="15.26953125" customWidth="1"/>
-    <col min="1794" max="1800" width="15.26953125" customWidth="1"/>
-    <col min="2050" max="2056" width="15.26953125" customWidth="1"/>
-    <col min="2306" max="2312" width="15.26953125" customWidth="1"/>
-    <col min="2562" max="2568" width="15.26953125" customWidth="1"/>
-    <col min="2818" max="2824" width="15.26953125" customWidth="1"/>
-    <col min="3074" max="3080" width="15.26953125" customWidth="1"/>
-    <col min="3330" max="3336" width="15.26953125" customWidth="1"/>
-    <col min="3586" max="3592" width="15.26953125" customWidth="1"/>
-    <col min="3842" max="3848" width="15.26953125" customWidth="1"/>
-    <col min="4098" max="4104" width="15.26953125" customWidth="1"/>
-    <col min="4354" max="4360" width="15.26953125" customWidth="1"/>
-    <col min="4610" max="4616" width="15.26953125" customWidth="1"/>
-    <col min="4866" max="4872" width="15.26953125" customWidth="1"/>
-    <col min="5122" max="5128" width="15.26953125" customWidth="1"/>
-    <col min="5378" max="5384" width="15.26953125" customWidth="1"/>
-    <col min="5634" max="5640" width="15.26953125" customWidth="1"/>
-    <col min="5890" max="5896" width="15.26953125" customWidth="1"/>
-    <col min="6146" max="6152" width="15.26953125" customWidth="1"/>
-    <col min="6402" max="6408" width="15.26953125" customWidth="1"/>
-    <col min="6658" max="6664" width="15.26953125" customWidth="1"/>
-    <col min="6914" max="6920" width="15.26953125" customWidth="1"/>
-    <col min="7170" max="7176" width="15.26953125" customWidth="1"/>
-    <col min="7426" max="7432" width="15.26953125" customWidth="1"/>
-    <col min="7682" max="7688" width="15.26953125" customWidth="1"/>
-    <col min="7938" max="7944" width="15.26953125" customWidth="1"/>
-    <col min="8194" max="8200" width="15.26953125" customWidth="1"/>
-    <col min="8450" max="8456" width="15.26953125" customWidth="1"/>
-    <col min="8706" max="8712" width="15.26953125" customWidth="1"/>
-    <col min="8962" max="8968" width="15.26953125" customWidth="1"/>
-    <col min="9218" max="9224" width="15.26953125" customWidth="1"/>
-    <col min="9474" max="9480" width="15.26953125" customWidth="1"/>
-    <col min="9730" max="9736" width="15.26953125" customWidth="1"/>
-    <col min="9986" max="9992" width="15.26953125" customWidth="1"/>
-    <col min="10242" max="10248" width="15.26953125" customWidth="1"/>
-    <col min="10498" max="10504" width="15.26953125" customWidth="1"/>
-    <col min="10754" max="10760" width="15.26953125" customWidth="1"/>
-    <col min="11010" max="11016" width="15.26953125" customWidth="1"/>
-    <col min="11266" max="11272" width="15.26953125" customWidth="1"/>
-    <col min="11522" max="11528" width="15.26953125" customWidth="1"/>
-    <col min="11778" max="11784" width="15.26953125" customWidth="1"/>
-    <col min="12034" max="12040" width="15.26953125" customWidth="1"/>
-    <col min="12290" max="12296" width="15.26953125" customWidth="1"/>
-    <col min="12546" max="12552" width="15.26953125" customWidth="1"/>
-    <col min="12802" max="12808" width="15.26953125" customWidth="1"/>
-    <col min="13058" max="13064" width="15.26953125" customWidth="1"/>
-    <col min="13314" max="13320" width="15.26953125" customWidth="1"/>
-    <col min="13570" max="13576" width="15.26953125" customWidth="1"/>
-    <col min="13826" max="13832" width="15.26953125" customWidth="1"/>
-    <col min="14082" max="14088" width="15.26953125" customWidth="1"/>
-    <col min="14338" max="14344" width="15.26953125" customWidth="1"/>
-    <col min="14594" max="14600" width="15.26953125" customWidth="1"/>
-    <col min="14850" max="14856" width="15.26953125" customWidth="1"/>
-    <col min="15106" max="15112" width="15.26953125" customWidth="1"/>
-    <col min="15362" max="15368" width="15.26953125" customWidth="1"/>
-    <col min="15618" max="15624" width="15.26953125" customWidth="1"/>
-    <col min="15874" max="15880" width="15.26953125" customWidth="1"/>
-    <col min="16130" max="16136" width="15.26953125" customWidth="1"/>
+    <col min="2" max="8" width="15.21875" customWidth="1"/>
+    <col min="258" max="264" width="15.21875" customWidth="1"/>
+    <col min="514" max="520" width="15.21875" customWidth="1"/>
+    <col min="770" max="776" width="15.21875" customWidth="1"/>
+    <col min="1026" max="1032" width="15.21875" customWidth="1"/>
+    <col min="1282" max="1288" width="15.21875" customWidth="1"/>
+    <col min="1538" max="1544" width="15.21875" customWidth="1"/>
+    <col min="1794" max="1800" width="15.21875" customWidth="1"/>
+    <col min="2050" max="2056" width="15.21875" customWidth="1"/>
+    <col min="2306" max="2312" width="15.21875" customWidth="1"/>
+    <col min="2562" max="2568" width="15.21875" customWidth="1"/>
+    <col min="2818" max="2824" width="15.21875" customWidth="1"/>
+    <col min="3074" max="3080" width="15.21875" customWidth="1"/>
+    <col min="3330" max="3336" width="15.21875" customWidth="1"/>
+    <col min="3586" max="3592" width="15.21875" customWidth="1"/>
+    <col min="3842" max="3848" width="15.21875" customWidth="1"/>
+    <col min="4098" max="4104" width="15.21875" customWidth="1"/>
+    <col min="4354" max="4360" width="15.21875" customWidth="1"/>
+    <col min="4610" max="4616" width="15.21875" customWidth="1"/>
+    <col min="4866" max="4872" width="15.21875" customWidth="1"/>
+    <col min="5122" max="5128" width="15.21875" customWidth="1"/>
+    <col min="5378" max="5384" width="15.21875" customWidth="1"/>
+    <col min="5634" max="5640" width="15.21875" customWidth="1"/>
+    <col min="5890" max="5896" width="15.21875" customWidth="1"/>
+    <col min="6146" max="6152" width="15.21875" customWidth="1"/>
+    <col min="6402" max="6408" width="15.21875" customWidth="1"/>
+    <col min="6658" max="6664" width="15.21875" customWidth="1"/>
+    <col min="6914" max="6920" width="15.21875" customWidth="1"/>
+    <col min="7170" max="7176" width="15.21875" customWidth="1"/>
+    <col min="7426" max="7432" width="15.21875" customWidth="1"/>
+    <col min="7682" max="7688" width="15.21875" customWidth="1"/>
+    <col min="7938" max="7944" width="15.21875" customWidth="1"/>
+    <col min="8194" max="8200" width="15.21875" customWidth="1"/>
+    <col min="8450" max="8456" width="15.21875" customWidth="1"/>
+    <col min="8706" max="8712" width="15.21875" customWidth="1"/>
+    <col min="8962" max="8968" width="15.21875" customWidth="1"/>
+    <col min="9218" max="9224" width="15.21875" customWidth="1"/>
+    <col min="9474" max="9480" width="15.21875" customWidth="1"/>
+    <col min="9730" max="9736" width="15.21875" customWidth="1"/>
+    <col min="9986" max="9992" width="15.21875" customWidth="1"/>
+    <col min="10242" max="10248" width="15.21875" customWidth="1"/>
+    <col min="10498" max="10504" width="15.21875" customWidth="1"/>
+    <col min="10754" max="10760" width="15.21875" customWidth="1"/>
+    <col min="11010" max="11016" width="15.21875" customWidth="1"/>
+    <col min="11266" max="11272" width="15.21875" customWidth="1"/>
+    <col min="11522" max="11528" width="15.21875" customWidth="1"/>
+    <col min="11778" max="11784" width="15.21875" customWidth="1"/>
+    <col min="12034" max="12040" width="15.21875" customWidth="1"/>
+    <col min="12290" max="12296" width="15.21875" customWidth="1"/>
+    <col min="12546" max="12552" width="15.21875" customWidth="1"/>
+    <col min="12802" max="12808" width="15.21875" customWidth="1"/>
+    <col min="13058" max="13064" width="15.21875" customWidth="1"/>
+    <col min="13314" max="13320" width="15.21875" customWidth="1"/>
+    <col min="13570" max="13576" width="15.21875" customWidth="1"/>
+    <col min="13826" max="13832" width="15.21875" customWidth="1"/>
+    <col min="14082" max="14088" width="15.21875" customWidth="1"/>
+    <col min="14338" max="14344" width="15.21875" customWidth="1"/>
+    <col min="14594" max="14600" width="15.21875" customWidth="1"/>
+    <col min="14850" max="14856" width="15.21875" customWidth="1"/>
+    <col min="15106" max="15112" width="15.21875" customWidth="1"/>
+    <col min="15362" max="15368" width="15.21875" customWidth="1"/>
+    <col min="15618" max="15624" width="15.21875" customWidth="1"/>
+    <col min="15874" max="15880" width="15.21875" customWidth="1"/>
+    <col min="16130" max="16136" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="25" t="s">
         <v>13</v>
       </c>
@@ -835,7 +838,7 @@
       <c r="G1" s="26"/>
       <c r="H1" s="27"/>
     </row>
-    <row r="2" spans="1:8" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -924,13 +927,15 @@
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="D7" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="21"/>
       <c r="H7" s="22"/>
     </row>
-    <row r="8" spans="1:8" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -1022,7 +1027,7 @@
       <c r="G13" s="21"/>
       <c r="H13" s="22"/>
     </row>
-    <row r="14" spans="1:8" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
@@ -1114,7 +1119,7 @@
       <c r="G19" s="21"/>
       <c r="H19" s="22"/>
     </row>
-    <row r="20" spans="1:8" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>12</v>
       </c>
@@ -1202,7 +1207,7 @@
       <c r="G25" s="21"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:8" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>12</v>
       </c>
@@ -1288,7 +1293,7 @@
       <c r="G31" s="11"/>
       <c r="H31" s="12"/>
     </row>
-    <row r="32" spans="1:8" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>12</v>
       </c>

</xml_diff>